<commit_message>
update country and fullloadtime
</commit_message>
<xml_diff>
--- a/data/Today_Demo_10122018.xlsx
+++ b/data/Today_Demo_10122018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>Urls</t>
   </si>
@@ -140,6 +140,33 @@
   </si>
   <si>
     <t>B(83%)</t>
+  </si>
+  <si>
+    <t>https://www.webpagetest.org/result/181212_8N_c0161381264f9588ff0459ef2f74f400/</t>
+  </si>
+  <si>
+    <t>3.67</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/yi4IXeUB</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/lT6KAKdi</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/6Aqr7907</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/wRv2WAmG</t>
+  </si>
+  <si>
+    <t>D(66%)</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/fLJQvGAB</t>
+  </si>
+  <si>
+    <t>https://gtmetrix.com/reports/www.sfwmd.gov/JAmjChrW</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1202,12 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
@@ -1368,7 +1399,7 @@
         <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>